<commit_message>
power measurement spreadsheet is now cleaner
 Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/Benchmarking/power mmt.xlsx
+++ b/Benchmarking/power mmt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Desktop/Grp Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/pocketReg/Benchmarking/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>power factor</t>
   </si>
@@ -72,13 +72,31 @@
   </si>
   <si>
     <t>scal mult</t>
+  </si>
+  <si>
+    <t>Parallela</t>
+  </si>
+  <si>
+    <t>Idle</t>
+  </si>
+  <si>
+    <t>Scalar Multiplication</t>
+  </si>
+  <si>
+    <t>Jettson TX1</t>
+  </si>
+  <si>
+    <t>Measurements of interest:</t>
+  </si>
+  <si>
+    <t>All measurements:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -90,6 +108,37 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,10 +210,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -178,8 +243,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -455,111 +541,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T17"/>
+  <dimension ref="B1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" style="10"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B1" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B2" s="9"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="13"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B3" s="9"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="B4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="17">
+        <v>6.6</v>
+      </c>
+      <c r="D4" s="13">
+        <v>7.4</v>
+      </c>
+      <c r="E4" s="17">
+        <v>3.1</v>
+      </c>
+      <c r="F4" s="13">
+        <v>5.3</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B5" s="9"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="B5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="17">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D5" s="13">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E5" s="17">
+        <v>3.9E-2</v>
+      </c>
+      <c r="F5" s="13">
+        <v>5.2999999999999999E-2</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="E7" s="6"/>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="6"/>
-    </row>
+    <row r="6" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B8" s="11"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -570,177 +647,247 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B9" s="12" t="s">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B11" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="E13" s="6"/>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B14" s="11"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B15" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3">
         <v>3120</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E15" s="8">
         <v>3120</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F15" s="3">
         <v>3120</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B10" s="9" t="s">
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1">
         <v>6.8</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E16" s="6">
         <v>6.6</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F16" s="1">
         <v>7.4</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G16" s="1">
         <v>7.4</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H16" s="1">
         <v>7.4</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I16" s="6">
         <v>3.1</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J16" s="4">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B11" s="9" t="s">
+      <c r="K16">
+        <f>J16/I16</f>
+        <v>1.7096774193548385</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1">
         <v>241.1</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
+      <c r="E17" s="6"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="1"/>
+      <c r="K17">
+        <f>F16/E16</f>
+        <v>1.1212121212121213</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1">
         <v>50</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E18" s="6">
         <v>50</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B13" s="9" t="s">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E19" s="6">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F19" s="1">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G19" s="1">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H19" s="1">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I19" s="6">
         <v>3.9E-2</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J19" s="4">
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B14" s="9" t="s">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1">
         <v>0.61</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E20" s="7">
         <v>0.43</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F20" s="1">
         <v>0.49</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G20" s="1">
         <v>0.49</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H20" s="1">
         <v>0.49</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I20" s="6">
         <v>0.43</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J20" s="4">
         <v>0.43</v>
       </c>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B15" s="9" t="s">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1">
         <v>21.8</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E21" s="7">
         <v>21.8</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B16" s="11" t="s">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2">
         <v>2</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E22" s="5">
         <v>2</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>